<commit_message>
Archivos de timbrado sa
</commit_message>
<xml_diff>
--- a/XurtepNominas/bin/Debug/Archivos/marinos1.xlsx
+++ b/XurtepNominas/bin/Debug/Archivos/marinos1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eduardo\Documents\MBC Group\Timbrado\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escritorio\Xurtep\XurtepNominas\XurtepNominas\bin\Debug\Archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -238,7 +238,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="82">
   <si>
     <t>No. Empleado</t>
   </si>
@@ -475,13 +475,22 @@
   </si>
   <si>
     <t>Tipo</t>
+  </si>
+  <si>
+    <t>94/002</t>
+  </si>
+  <si>
+    <t>SUBSIDIO</t>
+  </si>
+  <si>
+    <t>Subsidio Causado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -518,6 +527,12 @@
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Lucida Console"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -777,44 +792,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -826,15 +809,65 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1140,7 +1173,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:XFD267"/>
+      <selection pane="bottomRight" sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1173,85 +1206,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="9"/>
-      <c r="O1" s="12" t="s">
+      <c r="N1" s="16"/>
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="P1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="10" t="s">
+      <c r="Q1" s="16"/>
+      <c r="R1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="9"/>
-      <c r="T1" s="12" t="s">
+      <c r="S1" s="16"/>
+      <c r="T1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="12" t="s">
+      <c r="U1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="10" t="s">
+      <c r="V1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="W1" s="9"/>
-      <c r="X1" s="10" t="s">
+      <c r="W1" s="16"/>
+      <c r="X1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="Y1" s="9"/>
-      <c r="Z1" s="10" t="s">
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="AA1" s="9"/>
-      <c r="AB1" s="12" t="s">
+      <c r="AA1" s="16"/>
+      <c r="AB1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AC1" s="12" t="s">
+      <c r="AC1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AD1" s="12" t="s">
+      <c r="AD1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AE1" s="12" t="s">
+      <c r="AE1" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1278,236 +1311,243 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD270"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" customWidth="1"/>
     <col min="2" max="2" width="42.7109375" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="26"/>
+      <c r="E1" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="28"/>
+      <c r="G1" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="26"/>
+      <c r="I1" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="28"/>
+      <c r="K1" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" s="20"/>
-      <c r="G1" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" s="18"/>
-      <c r="I1" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="20"/>
-      <c r="K1" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="L1" s="18"/>
-      <c r="M1" s="19" t="s">
+      <c r="L1" s="26"/>
+      <c r="M1" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="N1" s="20"/>
-      <c r="O1" s="17" t="s">
+      <c r="N1" s="28"/>
+      <c r="O1" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="R1" s="20"/>
-      <c r="S1" s="17" t="s">
+      <c r="R1" s="26"/>
+      <c r="S1" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="T1" s="21"/>
-      <c r="U1" s="21"/>
-      <c r="V1" s="21"/>
-      <c r="W1" s="21"/>
-      <c r="X1" s="21"/>
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="19" t="s">
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="AA1" s="20"/>
-      <c r="AB1" s="17" t="s">
+      <c r="AA1" s="28"/>
+      <c r="AB1" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="AC1" s="18"/>
-      <c r="AD1" s="19" t="s">
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="AE1" s="20"/>
-      <c r="AF1" s="17" t="s">
+      <c r="AE1" s="28"/>
+      <c r="AF1" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="AG1" s="18"/>
+      <c r="AG1" s="26"/>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="31"/>
+      <c r="E2" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="33"/>
+      <c r="G2" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="31"/>
+      <c r="I2" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="33"/>
+      <c r="K2" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="J2" s="5"/>
-      <c r="K2" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="L2" s="7"/>
-      <c r="M2" s="6" t="s">
+      <c r="L2" s="31"/>
+      <c r="M2" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="N2" s="5"/>
-      <c r="O2" s="8" t="s">
+      <c r="N2" s="33"/>
+      <c r="O2" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="R2" s="5"/>
-      <c r="S2" s="8" t="s">
+      <c r="R2" s="31"/>
+      <c r="S2" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
-      <c r="Y2" s="7"/>
-      <c r="Z2" s="6" t="s">
+      <c r="T2" s="34"/>
+      <c r="U2" s="34"/>
+      <c r="V2" s="34"/>
+      <c r="W2" s="34"/>
+      <c r="X2" s="34"/>
+      <c r="Y2" s="31"/>
+      <c r="Z2" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="AA2" s="5"/>
-      <c r="AB2" s="8" t="s">
+      <c r="AA2" s="33"/>
+      <c r="AB2" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="AC2" s="7"/>
-      <c r="AD2" s="6" t="s">
+      <c r="AC2" s="31"/>
+      <c r="AD2" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="AE2" s="5"/>
-      <c r="AF2" s="8" t="s">
+      <c r="AE2" s="33"/>
+      <c r="AF2" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="AG2" s="7"/>
+      <c r="AG2" s="31"/>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="J3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="K3" s="14" t="s">
+      <c r="K3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="L3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="M3" s="14" t="s">
+      <c r="M3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="N3" s="15" t="s">
+      <c r="N3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="O3" s="14" t="s">
+      <c r="O3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="P3" s="15" t="s">
+      <c r="P3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="Q3" s="14" t="s">
+      <c r="Q3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="R3" s="15" t="s">
+      <c r="R3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="S3" s="14" t="s">
+      <c r="S3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="T3" s="16" t="s">
+      <c r="T3" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="U3" s="16" t="s">
+      <c r="U3" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="V3" s="16" t="s">
+      <c r="V3" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="W3" s="16" t="s">
+      <c r="W3" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="X3" s="16" t="s">
+      <c r="X3" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="Y3" s="15" t="s">
+      <c r="Y3" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="Z3" s="14" t="s">
+      <c r="Z3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="AA3" s="15" t="s">
+      <c r="AA3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="AB3" s="14" t="s">
+      <c r="AB3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="AC3" s="15" t="s">
+      <c r="AC3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="AD3" s="14" t="s">
+      <c r="AD3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="AE3" s="15" t="s">
+      <c r="AE3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="AF3" s="14" t="s">
+      <c r="AF3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="AG3" s="15" t="s">
+      <c r="AG3" s="4" t="s">
         <v>52</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
     <mergeCell ref="AB2:AC2"/>
     <mergeCell ref="AD2:AE2"/>
     <mergeCell ref="AF2:AG2"/>
@@ -1516,11 +1556,6 @@
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="S2:Y2"/>
     <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -1547,105 +1582,105 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="26"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="24" t="s">
+      <c r="G1" s="14"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="J1" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="K1" s="24" t="s">
+      <c r="K1" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="L1" s="25" t="s">
+      <c r="L1" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="M1" s="24" t="s">
+      <c r="M1" s="12" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="3" t="s">
+      <c r="G2" s="24"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="23" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="I3" s="22" t="s">
+      <c r="I3" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="J3" s="22" t="s">
+      <c r="J3" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="K3" s="22" t="s">
+      <c r="K3" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="L3" s="22" t="s">
+      <c r="L3" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="M3" s="22" t="s">
+      <c r="M3" s="10" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1668,17 +1703,52 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="34.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="7"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C2" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="19"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
 </file>
</xml_diff>